<commit_message>
upd: gost, apa, tests
</commit_message>
<xml_diff>
--- a/media/template.xlsx
+++ b/media/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelnv/python/course/module1/project/media/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python-course-bibliography-generator\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D214F9-F66B-194A-AA07-D1DE2931A26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2177336-CCA3-4E3E-A728-029B09110B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="760" windowWidth="32040" windowHeight="17440" xr2:uid="{1807092D-0DC2-8D42-BD0F-6967B3E6F74C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" firstSheet="2" activeTab="5" xr2:uid="{1807092D-0DC2-8D42-BD0F-6967B3E6F74C}"/>
   </bookViews>
   <sheets>
     <sheet name="Книга" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
   <si>
     <t>Фамилии и инициалы авторов</t>
   </si>
@@ -255,6 +255,12 @@
   </si>
   <si>
     <t>http://www.tapemark.narod.ru/les/index.html</t>
+  </si>
+  <si>
+    <t>doi</t>
+  </si>
+  <si>
+    <t>10.2196/16504</t>
   </si>
 </sst>
 </file>
@@ -316,7 +322,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -330,10 +336,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -344,11 +347,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Финансовый" xfId="2" builtinId="3"/>
   </cellStyles>
-  <dxfs count="71">
+  <dxfs count="73">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -576,136 +585,138 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{145AC3C6-38B1-A240-AC4B-92D1F879E94C}" name="Table1" displayName="Table1" ref="A1:G10" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
-  <autoFilter ref="A1:G10" xr:uid="{145AC3C6-38B1-A240-AC4B-92D1F879E94C}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AC8A8191-06B9-1441-BF8F-D1FFC678252E}" name="Фамилии и инициалы авторов" dataDxfId="68"/>
-    <tableColumn id="2" xr3:uid="{F350D718-7977-1F46-ACD7-0D83A59D5FBD}" name="Название книги" dataDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{243BA16D-ED2B-9E4F-AF91-0D72D837C058}" name="Номер издания" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{FCC82FE5-0D92-9846-B961-F17B686B3239}" name="Город издательства" dataDxfId="65"/>
-    <tableColumn id="5" xr3:uid="{B65B8FC7-3724-0A4C-818A-AD7FA2AD64EB}" name="Название издательства" dataDxfId="64"/>
-    <tableColumn id="6" xr3:uid="{3BF7551B-0910-6F4D-9B33-0596C85F2318}" name="Год издания" dataDxfId="63"/>
-    <tableColumn id="7" xr3:uid="{AD55AB3E-21B8-9942-BD66-2174D1F429F3}" name="Количество страниц" dataDxfId="62"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{145AC3C6-38B1-A240-AC4B-92D1F879E94C}" name="Table1" displayName="Table1" ref="A1:H10" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+  <autoFilter ref="A1:H10" xr:uid="{145AC3C6-38B1-A240-AC4B-92D1F879E94C}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{AC8A8191-06B9-1441-BF8F-D1FFC678252E}" name="Фамилии и инициалы авторов" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{F350D718-7977-1F46-ACD7-0D83A59D5FBD}" name="Название книги" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{243BA16D-ED2B-9E4F-AF91-0D72D837C058}" name="Номер издания" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{FCC82FE5-0D92-9846-B961-F17B686B3239}" name="Город издательства" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{B65B8FC7-3724-0A4C-818A-AD7FA2AD64EB}" name="Название издательства" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{3BF7551B-0910-6F4D-9B33-0596C85F2318}" name="Год издания" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{AD55AB3E-21B8-9942-BD66-2174D1F429F3}" name="Количество страниц" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{3DFCC7DE-2DCA-4194-8174-CA8A881F0389}" name="doi" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D355B9CA-7CD4-8A41-92BA-C40FCDFDB994}" name="Table13" displayName="Table13" ref="A1:D10" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D355B9CA-7CD4-8A41-92BA-C40FCDFDB994}" name="Table13" displayName="Table13" ref="A1:D10" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
   <autoFilter ref="A1:D10" xr:uid="{D355B9CA-7CD4-8A41-92BA-C40FCDFDB994}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D476E401-D70E-874A-B348-D15B3214EC91}" name="Заголовок статьи или страницы" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{C1DEDF42-6C25-244E-939A-FE8A4F312488}" name="Название сайта" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{26730401-FB4F-2647-92F2-A74F4F5D4F9D}" name="Гиперссылка" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{C1B155B8-9134-2546-98E6-69F88F344657}" name="Дата обращения на сайт" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{D476E401-D70E-874A-B348-D15B3214EC91}" name="Заголовок статьи или страницы" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{C1DEDF42-6C25-244E-939A-FE8A4F312488}" name="Название сайта" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{26730401-FB4F-2647-92F2-A74F4F5D4F9D}" name="Гиперссылка" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{C1B155B8-9134-2546-98E6-69F88F344657}" name="Дата обращения на сайт" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DB4EAEF-7DA6-BF45-829D-A22C9344355B}" name="Table14" displayName="Table14" ref="A1:I10" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DB4EAEF-7DA6-BF45-829D-A22C9344355B}" name="Table14" displayName="Table14" ref="A1:I10" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
   <autoFilter ref="A1:I10" xr:uid="{7DB4EAEF-7DA6-BF45-829D-A22C9344355B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{DA93F8CE-55DD-D743-BCEE-9232685F043C}" name="Тип нормативного актa" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{9BB8859E-564C-9846-8E2C-1E22DB3472BF}" name="Полное название нормативного акта" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{50ADE570-C0CD-2B41-9BDF-CC06F4CC9831}" name="Дата принятия" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{C07BB0E4-B237-C04C-BA14-2D73F0218063}" name="Номер нормативного акта" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{0B6FDCAC-52DF-4F44-BB09-CD5C24FE78A4}" name="Официальный источник опубликования" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{BDB655D3-D12C-8F4B-92F0-83137AC7E6CA}" name="Год публикации источника" dataDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{0B4C92C5-1F56-D840-8F44-FF7CA414CFF9}" name="Номер выхода источника" dataDxfId="47"/>
-    <tableColumn id="8" xr3:uid="{B1CAC8DB-A933-A549-BD80-E5454D60F720}" name="Номер статьи" dataDxfId="46"/>
-    <tableColumn id="9" xr3:uid="{A667D7F7-BF79-4842-A8E6-2E7475B3BFDA}" name="В редакции от" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{DA93F8CE-55DD-D743-BCEE-9232685F043C}" name="Тип нормативного актa" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{9BB8859E-564C-9846-8E2C-1E22DB3472BF}" name="Полное название нормативного акта" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{50ADE570-C0CD-2B41-9BDF-CC06F4CC9831}" name="Дата принятия" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{C07BB0E4-B237-C04C-BA14-2D73F0218063}" name="Номер нормативного акта" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{0B6FDCAC-52DF-4F44-BB09-CD5C24FE78A4}" name="Официальный источник опубликования" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{BDB655D3-D12C-8F4B-92F0-83137AC7E6CA}" name="Год публикации источника" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{0B4C92C5-1F56-D840-8F44-FF7CA414CFF9}" name="Номер выхода источника" dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{B1CAC8DB-A933-A549-BD80-E5454D60F720}" name="Номер статьи" dataDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{A667D7F7-BF79-4842-A8E6-2E7475B3BFDA}" name="В редакции от" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{94289CB7-CAB4-4B41-906A-C57ECC3ABC4F}" name="Table145" displayName="Table145" ref="A1:H10" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{94289CB7-CAB4-4B41-906A-C57ECC3ABC4F}" name="Table145" displayName="Table145" ref="A1:H10" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:H10" xr:uid="{94289CB7-CAB4-4B41-906A-C57ECC3ABC4F}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{0F8BA47B-7AAA-E84B-9156-115C2EEEA3B0}" name="Фамилия и инициалы автора" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{CAEF0393-8E3E-B648-A5EC-C0F6FCF1327D}" name="Название диссертации" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{74943D0B-8368-FF41-9D34-F317958490F2}" name="Доктора или кандидата" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{C4315642-C99E-D64C-A95E-97973935750C}" name="Отрасль наук (сокращённо)" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{6C48EAEB-038A-8543-9C05-4B820CD991C0}" name="Код специальности" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{B6B80C0D-F76C-BB4B-810E-80C0B25B79E8}" name="Город издательства" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{51352836-93D1-0244-B976-3D400D44A6D9}" name="Год" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{6C20AF3C-B5E2-4C4F-8F27-D30ED97E66FA}" name="Количество страниц" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{0F8BA47B-7AAA-E84B-9156-115C2EEEA3B0}" name="Фамилия и инициалы автора" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{CAEF0393-8E3E-B648-A5EC-C0F6FCF1327D}" name="Название диссертации" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{74943D0B-8368-FF41-9D34-F317958490F2}" name="Доктора или кандидата" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{C4315642-C99E-D64C-A95E-97973935750C}" name="Отрасль наук (сокращённо)" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{6C48EAEB-038A-8543-9C05-4B820CD991C0}" name="Код специальности" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{B6B80C0D-F76C-BB4B-810E-80C0B25B79E8}" name="Город издательства" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{51352836-93D1-0244-B976-3D400D44A6D9}" name="Год" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{6C20AF3C-B5E2-4C4F-8F27-D30ED97E66FA}" name="Количество страниц" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{72406609-A584-6C45-BF44-96788CEB6AEC}" name="Table1457" displayName="Table1457" ref="A1:H10" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{72406609-A584-6C45-BF44-96788CEB6AEC}" name="Table1457" displayName="Table1457" ref="A1:H10" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="A1:H10" xr:uid="{72406609-A584-6C45-BF44-96788CEB6AEC}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{218AD14A-262B-EA4C-AECA-73E3B893ED02}" name="Фамилия и инициалы автора" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{49D78B99-20BD-5F46-A905-B9B1B291B9D3}" name="Название диссертации" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{B4B6E55D-2DDB-224C-8E95-F8ADCA1FB8DF}" name="Доктора или кандидата" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{D2DE7460-934C-4942-A044-36E157712657}" name="Отрасль наук (сокращённо)" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{008B47C9-18AD-F64C-B7B4-CF84E16603EB}" name="Код специальности" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{74CFE771-7D58-D449-9872-A92BEC84404A}" name="Город издательства" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{A66A001C-F244-AF49-85A8-49BEA05AEFF3}" name="Год" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{FA5C95CD-621E-5A45-B488-3CDD323AC491}" name="Количество страниц" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{218AD14A-262B-EA4C-AECA-73E3B893ED02}" name="Фамилия и инициалы автора" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{49D78B99-20BD-5F46-A905-B9B1B291B9D3}" name="Название диссертации" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{B4B6E55D-2DDB-224C-8E95-F8ADCA1FB8DF}" name="Доктора или кандидата" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{D2DE7460-934C-4942-A044-36E157712657}" name="Отрасль наук (сокращённо)" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{008B47C9-18AD-F64C-B7B4-CF84E16603EB}" name="Код специальности" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{74CFE771-7D58-D449-9872-A92BEC84404A}" name="Город издательства" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{A66A001C-F244-AF49-85A8-49BEA05AEFF3}" name="Год" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{FA5C95CD-621E-5A45-B488-3CDD323AC491}" name="Количество страниц" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{0DE3887D-FC43-4642-90F3-B3B1CDB3B1E2}" name="Table14578" displayName="Table14578" ref="A1:F10" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A1:F10" xr:uid="{0DE3887D-FC43-4642-90F3-B3B1CDB3B1E2}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E85F3D3F-BDAD-CC4C-8B9D-B391E38977AD}" name="Фамилии и инициалы авторов" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{E6649EE8-B26D-5444-9FBE-9A6423CE741D}" name="Название статьи" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{E6FE16AD-7A63-3144-94B4-55B3D4746E28}" name="Название журнала" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{2CB4E4B6-F265-2343-B009-02C3DBE93DC0}" name="Год издания" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{D3969755-95DC-3B45-B7B6-617194750EFA}" name="Номер журнала" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{A44563D1-DB78-D547-8F47-1615C0651EFE}" name="Страницы статьи в журнале" dataDxfId="17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{0DE3887D-FC43-4642-90F3-B3B1CDB3B1E2}" name="Table14578" displayName="Table14578" ref="A1:G10" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+  <autoFilter ref="A1:G10" xr:uid="{0DE3887D-FC43-4642-90F3-B3B1CDB3B1E2}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{E85F3D3F-BDAD-CC4C-8B9D-B391E38977AD}" name="Фамилии и инициалы авторов" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{E6649EE8-B26D-5444-9FBE-9A6423CE741D}" name="Название статьи" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{E6FE16AD-7A63-3144-94B4-55B3D4746E28}" name="Название журнала" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{2CB4E4B6-F265-2343-B009-02C3DBE93DC0}" name="Год издания" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{D3969755-95DC-3B45-B7B6-617194750EFA}" name="Номер журнала" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{A44563D1-DB78-D547-8F47-1615C0651EFE}" name="Страницы статьи в журнале" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{C4B089A4-5ACA-4958-A248-F50D017BA825}" name="doi" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8CF07A18-ACC5-F24E-92CF-2BCBADB418DD}" name="Table145789" displayName="Table145789" ref="A1:G10" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8CF07A18-ACC5-F24E-92CF-2BCBADB418DD}" name="Table145789" displayName="Table145789" ref="A1:G10" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A1:G10" xr:uid="{8CF07A18-ACC5-F24E-92CF-2BCBADB418DD}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{4D09D55E-1107-7B47-B370-7D852543B864}" name="Фамилии и инициалы авторов" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{658A8A15-22FA-D147-A8AC-985FFC9CB0D1}" name="Название статьи" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{81DBBD20-B380-3542-8736-317B25A122BB}" name="Название сборника" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{597B51F8-A03B-8345-824F-D7940CB464C5}" name="Город издательства" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{DB6499B6-3347-5146-9C7A-618D05375681}" name="Название издательства" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{F2F08906-1C92-6C44-BF7B-4A64D1CB0AC5}" name="Год издания" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{0FAFBE1C-CE60-A745-AA54-D007EE867899}" name="Страницы статьи в сборнике" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{4D09D55E-1107-7B47-B370-7D852543B864}" name="Фамилии и инициалы авторов" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{658A8A15-22FA-D147-A8AC-985FFC9CB0D1}" name="Название статьи" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{81DBBD20-B380-3542-8736-317B25A122BB}" name="Название сборника" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{597B51F8-A03B-8345-824F-D7940CB464C5}" name="Город издательства" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{DB6499B6-3347-5146-9C7A-618D05375681}" name="Название издательства" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{F2F08906-1C92-6C44-BF7B-4A64D1CB0AC5}" name="Год издания" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{0FAFBE1C-CE60-A745-AA54-D007EE867899}" name="Страницы статьи в сборнике" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{8249D061-41B8-6542-80FC-8E28B42526EE}" name="Table14578910" displayName="Table14578910" ref="A1:F10" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{8249D061-41B8-6542-80FC-8E28B42526EE}" name="Table14578910" displayName="Table14578910" ref="A1:F10" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:F10" xr:uid="{8249D061-41B8-6542-80FC-8E28B42526EE}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{50DB5770-807C-2945-BEE2-319304CB1204}" name="Фамилии и инициалы авторов" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{E22A958C-7018-BE4A-ACBA-CEFF7305EB84}" name="Название статьи" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{22E33630-897E-734D-B022-6DC572D1F5F8}" name="Название газеты" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{FC3C28B8-1372-9045-9DDA-4CA25260DF08}" name="Год издания" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{E60C91B3-331D-D147-BB31-DA99F6C069D7}" name="Дата выхода газеты" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{18333EC5-E6B7-5140-9D18-088CE78FD8D4}" name="Номер статьи" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{50DB5770-807C-2945-BEE2-319304CB1204}" name="Фамилии и инициалы авторов" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{E22A958C-7018-BE4A-ACBA-CEFF7305EB84}" name="Название статьи" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{22E33630-897E-734D-B022-6DC572D1F5F8}" name="Название газеты" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{FC3C28B8-1372-9045-9DDA-4CA25260DF08}" name="Год издания" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{E60C91B3-331D-D147-BB31-DA99F6C069D7}" name="Дата выхода газеты" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{18333EC5-E6B7-5140-9D18-088CE78FD8D4}" name="Номер статьи" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -743,7 +754,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -849,7 +860,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -999,13 +1010,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9485DB95-4C34-684F-A5A5-455A0D71C5A5}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
     <col min="2" max="2" width="44.83203125" customWidth="1"/>
@@ -1014,9 +1025,10 @@
     <col min="5" max="5" width="32.6640625" customWidth="1"/>
     <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1038,8 +1050,11 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H1" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1061,8 +1076,11 @@
       <c r="G2" s="2">
         <v>999</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H2" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>54</v>
       </c>
@@ -1084,8 +1102,9 @@
       <c r="G3" s="2">
         <v>360</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
@@ -1105,8 +1124,9 @@
       <c r="G4" s="2">
         <v>290</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>62</v>
       </c>
@@ -1126,8 +1146,9 @@
       <c r="G5" s="2">
         <v>624</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1135,8 +1156,9 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1144,8 +1166,9 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1153,8 +1176,9 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1162,8 +1186,9 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1171,8 +1196,9 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1197,7 +1223,7 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="46.1640625" customWidth="1"/>
     <col min="2" max="2" width="53.1640625" customWidth="1"/>
@@ -1205,7 +1231,7 @@
     <col min="4" max="4" width="25.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -1219,7 +1245,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1233,7 +1259,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>65</v>
       </c>
@@ -1247,51 +1273,51 @@
         <v>44206</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>70</v>
       </c>
       <c r="D4" s="4">
         <v>44197</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1318,7 +1344,7 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
     <col min="2" max="2" width="44.6640625" customWidth="1"/>
@@ -1331,7 +1357,7 @@
     <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -1360,7 +1386,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -1389,7 +1415,7 @@
         <v>37510</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1400,7 +1426,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1411,7 +1437,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1422,7 +1448,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1433,7 +1459,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1444,7 +1470,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1455,7 +1481,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1466,7 +1492,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1490,11 +1516,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA460EB4-94E1-174E-88D1-126827D78EC4}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35.83203125" customWidth="1"/>
     <col min="2" max="2" width="59.5" customWidth="1"/>
@@ -1506,7 +1532,7 @@
     <col min="8" max="8" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1532,20 +1558,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1558,7 +1584,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1568,7 +1594,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1578,7 +1604,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1588,7 +1614,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1598,7 +1624,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1608,7 +1634,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1618,7 +1644,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1628,7 +1654,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1653,11 +1679,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF624E0E-7143-2E45-B88B-583316D26BE9}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
     <col min="2" max="2" width="49.33203125" customWidth="1"/>
@@ -1669,7 +1695,7 @@
     <col min="8" max="8" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1695,20 +1721,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1721,7 +1747,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1731,7 +1757,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1741,7 +1767,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1751,7 +1777,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1761,7 +1787,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1771,7 +1797,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1781,7 +1807,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1791,7 +1817,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1814,13 +1840,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC7E9FB1-1298-B140-9EF8-6885E26C027A}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="37.83203125" customWidth="1"/>
     <col min="2" max="2" width="54" customWidth="1"/>
@@ -1828,9 +1854,10 @@
     <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1849,90 +1876,104 @@
       <c r="F1" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G1" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D2" s="2">
         <v>2020</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1950,7 +1991,7 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="40.33203125" customWidth="1"/>
     <col min="2" max="2" width="42.6640625" customWidth="1"/>
@@ -1961,7 +2002,7 @@
     <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1984,30 +2025,30 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="2">
         <v>2020</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2016,7 +2057,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2025,7 +2066,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2034,7 +2075,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2043,7 +2084,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2052,7 +2093,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2061,7 +2102,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2070,7 +2111,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2095,7 +2136,7 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="34.5" customWidth="1"/>
     <col min="2" max="2" width="36.5" customWidth="1"/>
@@ -2105,7 +2146,7 @@
     <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2125,27 +2166,27 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D2" s="2">
         <v>1980</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2153,7 +2194,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2161,7 +2202,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2169,7 +2210,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2177,7 +2218,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2185,7 +2226,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2193,7 +2234,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2201,7 +2242,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>

</xml_diff>